<commit_message>
update FS final D17 DST list
</commit_message>
<xml_diff>
--- a/cdw_tallyAnalysis/fopsFinal/D17_dstTallyAbundance.xlsx
+++ b/cdw_tallyAnalysis/fopsFinal/D17_dstTallyAbundance.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmeier/Documents/neonScienceDocs/gitRepositories/neonPlantSampling/cdw_tally_analysis/D17/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\neon-plant-sampling\cdw_tallyAnalysis\fopsFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D42A1834-8A7F-498F-AC2B-5B7E19C3DE1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="8863" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SJER BD DST rank" sheetId="1" r:id="rId1"/>
+    <sheet name="SOAP BD DST rank" sheetId="2" r:id="rId2"/>
+    <sheet name="TEAK BD DST rank" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="34">
   <si>
     <t>siteid</t>
   </si>
@@ -66,12 +69,75 @@
   </si>
   <si>
     <t>QUDO</t>
+  </si>
+  <si>
+    <t>siteID</t>
+  </si>
+  <si>
+    <t>taxonID</t>
+  </si>
+  <si>
+    <t>TEAK</t>
+  </si>
+  <si>
+    <t>ABMA</t>
+  </si>
+  <si>
+    <t>ABCO</t>
+  </si>
+  <si>
+    <t>PICO</t>
+  </si>
+  <si>
+    <t>2PLANT-H</t>
+  </si>
+  <si>
+    <t>PIJE</t>
+  </si>
+  <si>
+    <t>charextent</t>
+  </si>
+  <si>
+    <t>chardepth</t>
+  </si>
+  <si>
+    <t>SOAP</t>
+  </si>
+  <si>
+    <t>PIPO</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>PINUS</t>
+  </si>
+  <si>
+    <t>CADE27</t>
+  </si>
+  <si>
+    <t>1-5</t>
+  </si>
+  <si>
+    <t>0-1</t>
+  </si>
+  <si>
+    <t>6-25</t>
+  </si>
+  <si>
+    <t>QUKE</t>
+  </si>
+  <si>
+    <t>26-50</t>
+  </si>
+  <si>
+    <t>51-75</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -112,6 +178,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -379,26 +448,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.35546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.35546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.35546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.35546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -424,7 +493,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -450,7 +519,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -476,7 +545,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -502,7 +571,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -528,7 +597,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -554,7 +623,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -580,7 +649,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -606,7 +675,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -630,6 +699,1169 @@
       </c>
       <c r="H9">
         <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD0C1BB2-66A5-4B6C-9904-C68661A61C9D}">
+  <dimension ref="A1:J23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2">
+        <v>21.19</v>
+      </c>
+      <c r="H2">
+        <v>21.19</v>
+      </c>
+      <c r="I2">
+        <v>10</v>
+      </c>
+      <c r="J2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3">
+        <v>18.59</v>
+      </c>
+      <c r="H3">
+        <v>39.78</v>
+      </c>
+      <c r="I3">
+        <v>10</v>
+      </c>
+      <c r="J3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4">
+        <v>9.2899999999999991</v>
+      </c>
+      <c r="H4">
+        <v>49.07</v>
+      </c>
+      <c r="I4">
+        <v>10</v>
+      </c>
+      <c r="J4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5">
+        <v>4.09</v>
+      </c>
+      <c r="H5">
+        <v>53.16</v>
+      </c>
+      <c r="I5">
+        <v>10</v>
+      </c>
+      <c r="J5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6">
+        <v>2.6</v>
+      </c>
+      <c r="H6">
+        <v>55.76</v>
+      </c>
+      <c r="I6">
+        <v>10</v>
+      </c>
+      <c r="J6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7">
+        <v>2.23</v>
+      </c>
+      <c r="H7">
+        <v>57.99</v>
+      </c>
+      <c r="I7">
+        <v>10</v>
+      </c>
+      <c r="J7">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8">
+        <v>2.23</v>
+      </c>
+      <c r="H8">
+        <v>60.22</v>
+      </c>
+      <c r="I8">
+        <v>10</v>
+      </c>
+      <c r="J8">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9">
+        <v>2.23</v>
+      </c>
+      <c r="H9">
+        <v>62.45</v>
+      </c>
+      <c r="I9">
+        <v>10</v>
+      </c>
+      <c r="J9">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10">
+        <v>1.86</v>
+      </c>
+      <c r="H10">
+        <v>64.31</v>
+      </c>
+      <c r="I10">
+        <v>10</v>
+      </c>
+      <c r="J10">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11">
+        <v>1.86</v>
+      </c>
+      <c r="H11">
+        <v>66.17</v>
+      </c>
+      <c r="I11">
+        <v>10</v>
+      </c>
+      <c r="J11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12">
+        <v>1.49</v>
+      </c>
+      <c r="H12">
+        <v>67.66</v>
+      </c>
+      <c r="I12">
+        <v>10</v>
+      </c>
+      <c r="J12">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13">
+        <v>1.49</v>
+      </c>
+      <c r="H13">
+        <v>69.150000000000006</v>
+      </c>
+      <c r="I13">
+        <v>10</v>
+      </c>
+      <c r="J13">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14">
+        <v>1.49</v>
+      </c>
+      <c r="H14">
+        <v>70.64</v>
+      </c>
+      <c r="I14">
+        <v>10</v>
+      </c>
+      <c r="J14">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15">
+        <v>1.49</v>
+      </c>
+      <c r="H15">
+        <v>72.13</v>
+      </c>
+      <c r="I15">
+        <v>10</v>
+      </c>
+      <c r="J15">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="H16">
+        <v>73.25</v>
+      </c>
+      <c r="I16">
+        <v>10</v>
+      </c>
+      <c r="J16">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="H17">
+        <v>74.37</v>
+      </c>
+      <c r="I17">
+        <v>10</v>
+      </c>
+      <c r="J17">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="H18">
+        <v>75.489999999999995</v>
+      </c>
+      <c r="I18">
+        <v>10</v>
+      </c>
+      <c r="J18">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="H19">
+        <v>76.61</v>
+      </c>
+      <c r="I19">
+        <v>10</v>
+      </c>
+      <c r="J19">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20">
+        <v>0.74</v>
+      </c>
+      <c r="H20">
+        <v>77.349999999999994</v>
+      </c>
+      <c r="I20">
+        <v>10</v>
+      </c>
+      <c r="J20">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21">
+        <v>0.74</v>
+      </c>
+      <c r="H21">
+        <v>78.09</v>
+      </c>
+      <c r="I21">
+        <v>10</v>
+      </c>
+      <c r="J21">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22" t="s">
+        <v>29</v>
+      </c>
+      <c r="G22">
+        <v>0.74</v>
+      </c>
+      <c r="H22">
+        <v>78.83</v>
+      </c>
+      <c r="I22">
+        <v>10</v>
+      </c>
+      <c r="J22">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23">
+        <v>0.74</v>
+      </c>
+      <c r="H23">
+        <v>79.569999999999993</v>
+      </c>
+      <c r="I23">
+        <v>10</v>
+      </c>
+      <c r="J23">
+        <v>220</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93078230-C75A-4A43-AD10-25BACFE7CA28}">
+  <dimension ref="A1:H15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="3" width="9.5" customWidth="1"/>
+    <col min="4" max="4" width="11.640625" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="19.78515625" customWidth="1"/>
+    <col min="7" max="7" width="16.2109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>17.79</v>
+      </c>
+      <c r="F2">
+        <v>17.79</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>13.43</v>
+      </c>
+      <c r="F3">
+        <v>31.22</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>6.72</v>
+      </c>
+      <c r="F4">
+        <v>37.94</v>
+      </c>
+      <c r="G4">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <v>5.99</v>
+      </c>
+      <c r="F5">
+        <v>43.93</v>
+      </c>
+      <c r="G5">
+        <v>10</v>
+      </c>
+      <c r="H5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>5.81</v>
+      </c>
+      <c r="F6">
+        <v>49.74</v>
+      </c>
+      <c r="G6">
+        <v>10</v>
+      </c>
+      <c r="H6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>4.72</v>
+      </c>
+      <c r="F7">
+        <v>54.46</v>
+      </c>
+      <c r="G7">
+        <v>10</v>
+      </c>
+      <c r="H7">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <v>3.81</v>
+      </c>
+      <c r="F8">
+        <v>58.27</v>
+      </c>
+      <c r="G8">
+        <v>10</v>
+      </c>
+      <c r="H8">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>3.63</v>
+      </c>
+      <c r="F9">
+        <v>61.9</v>
+      </c>
+      <c r="G9">
+        <v>10</v>
+      </c>
+      <c r="H9">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>3.45</v>
+      </c>
+      <c r="F10">
+        <v>65.349999999999994</v>
+      </c>
+      <c r="G10">
+        <v>10</v>
+      </c>
+      <c r="H10">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>3.27</v>
+      </c>
+      <c r="F11">
+        <v>68.62</v>
+      </c>
+      <c r="G11">
+        <v>10</v>
+      </c>
+      <c r="H11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12">
+        <v>3.27</v>
+      </c>
+      <c r="F12">
+        <v>71.89</v>
+      </c>
+      <c r="G12">
+        <v>10</v>
+      </c>
+      <c r="H12">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13">
+        <v>2.9</v>
+      </c>
+      <c r="F13">
+        <v>74.790000000000006</v>
+      </c>
+      <c r="G13">
+        <v>10</v>
+      </c>
+      <c r="H13">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14">
+        <v>2.36</v>
+      </c>
+      <c r="F14">
+        <v>77.150000000000006</v>
+      </c>
+      <c r="G14">
+        <v>10</v>
+      </c>
+      <c r="H14">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15">
+        <v>2.36</v>
+      </c>
+      <c r="F15">
+        <v>79.510000000000005</v>
+      </c>
+      <c r="G15">
+        <v>10</v>
+      </c>
+      <c r="H15">
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>